<commit_message>
neue messreihe, neue matlab funktionen zur präzsisionserhöung von S, Power2 erweitert sendet jetzt alle berechneten Daten
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>R1</t>
   </si>
@@ -65,6 +65,42 @@
   </si>
   <si>
     <t>Neue Messreihe R1 alternierend, Spannungsteiler 18K 570</t>
+  </si>
+  <si>
+    <t>Rges</t>
+  </si>
+  <si>
+    <t>Sges</t>
+  </si>
+  <si>
+    <t>Inf</t>
+  </si>
+  <si>
+    <t>M05</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>18K</t>
+  </si>
+  <si>
+    <t>33K</t>
+  </si>
+  <si>
+    <t>R2 / Ω</t>
+  </si>
+  <si>
+    <t>R1 / Ω</t>
+  </si>
+  <si>
+    <t>Fs / Hz</t>
+  </si>
+  <si>
+    <t>Wie M04 nur andere Fs</t>
   </si>
 </sst>
 </file>
@@ -406,46 +442,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>561</v>
+      </c>
+      <c r="H2">
+        <f>(1/G2)</f>
+        <v>1.7825311942959001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>68.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:I12" si="0">(1/G3)</f>
+        <v>1.4598540145985401E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>61</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>1.6393442622950821E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>34.9</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.865329512893983E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -455,8 +525,15 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>3.0487804878048783E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -466,8 +543,15 @@
       <c r="D7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>23.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>4.2553191489361701E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -480,8 +564,15 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>22.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -494,8 +585,15 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>17.7</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>5.6497175141242938E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -511,8 +609,15 @@
       <c r="E10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>17.2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5.8139534883720929E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -528,8 +633,15 @@
       <c r="F11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>14.1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>7.0921985815602842E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -548,50 +660,133 @@
       <c r="F12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>13.8</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>7.2463768115942032E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>1000</v>
+      </c>
+      <c r="E19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>1000</v>
+      </c>
+      <c r="E20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>570</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+      <c r="E21" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>570</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Messung der berechneten Leistungswerte vom MC nun möglich, erste Messung D01 angelegt
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>R1</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Wie M04 nur andere Fs</t>
+  </si>
+  <si>
+    <t>M06</t>
+  </si>
+  <si>
+    <t>I wieder zurück gedreht, Shunt war überbrückt, jetzt mehr Spannung an ADC1, aber 180° verdreht</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>Messung und Berechnung durch den µC, Übertragung der Leistungsdaten</t>
   </si>
 </sst>
 </file>
@@ -442,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +493,7 @@
         <v>68.5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:I12" si="0">(1/G3)</f>
+        <f t="shared" ref="H3:H12" si="0">(1/G3)</f>
         <v>1.4598540145985401E-2</v>
       </c>
     </row>
@@ -783,6 +795,40 @@
       </c>
       <c r="E22" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>570</v>
+      </c>
+      <c r="D23">
+        <v>500</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>570</v>
+      </c>
+      <c r="D26">
+        <v>500</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neue messreihen mit und ohne Verstärker
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>R1</t>
   </si>
@@ -112,7 +112,25 @@
     <t>D01</t>
   </si>
   <si>
-    <t>Messung und Berechnung durch den µC, Übertragung der Leistungsdaten</t>
+    <t>M07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i_temp wird nun im Porgamm negativ berechnet </t>
+  </si>
+  <si>
+    <t>Verstärker</t>
+  </si>
+  <si>
+    <t>ohne</t>
+  </si>
+  <si>
+    <t>Messung und Berechnung durch den µC, Übertragung der Leistungsdaten (Ref: M06)</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>Berechnete Leisuntgsdaten mit vorher gedrehtem Vorzeichen von i_temp (Ref: M07)</t>
   </si>
 </sst>
 </file>
@@ -454,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
@@ -709,10 +727,13 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -726,10 +747,13 @@
         <v>1000</v>
       </c>
       <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -743,10 +767,13 @@
         <v>1000</v>
       </c>
       <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -760,10 +787,13 @@
         <v>1000</v>
       </c>
       <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -777,10 +807,13 @@
         <v>1000</v>
       </c>
       <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -794,10 +827,13 @@
         <v>500</v>
       </c>
       <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -811,10 +847,33 @@
         <v>500</v>
       </c>
       <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>570</v>
+      </c>
+      <c r="D24">
+        <v>500</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -828,7 +887,30 @@
         <v>500</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>570</v>
+      </c>
+      <c r="D27">
+        <v>500</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neue Messreihen D umbenannt sodass sie zu M passen D06->M06, neue Matlab Funktionen signalFFT.m, analyseHilbert.m
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
   <si>
     <t>R1</t>
   </si>
@@ -109,9 +109,6 @@
     <t>I wieder zurück gedreht, Shunt war überbrückt, jetzt mehr Spannung an ADC1, aber 180° verdreht</t>
   </si>
   <si>
-    <t>D01</t>
-  </si>
-  <si>
     <t>M07</t>
   </si>
   <si>
@@ -124,13 +121,82 @@
     <t>ohne</t>
   </si>
   <si>
-    <t>Messung und Berechnung durch den µC, Übertragung der Leistungsdaten (Ref: M06)</t>
-  </si>
-  <si>
-    <t>D02</t>
-  </si>
-  <si>
-    <t>Berechnete Leisuntgsdaten mit vorher gedrehtem Vorzeichen von i_temp (Ref: M07)</t>
+    <t>Versorgung</t>
+  </si>
+  <si>
+    <t>Schaltnetzteil</t>
+  </si>
+  <si>
+    <t>M08</t>
+  </si>
+  <si>
+    <t>gleich M07</t>
+  </si>
+  <si>
+    <t>M09</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>invertierender Verstärker</t>
+  </si>
+  <si>
+    <t>nicht-invertierender Verstärker und -i_temp, Übersteuern von i!</t>
+  </si>
+  <si>
+    <t>invertierender Verstärker, Übersteuern von i bei Messung 12</t>
+  </si>
+  <si>
+    <t>nicht-invertierender Verstärker und -i_temp, Übersteuern von i ab Messung 11!</t>
+  </si>
+  <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>D07</t>
+  </si>
+  <si>
+    <t>D08</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>ohne Versträker</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D09</t>
+  </si>
+  <si>
+    <t>Messung und Berechnung durch den µC, Übertragung der Leistungsdaten</t>
+  </si>
+  <si>
+    <t>Berechnete Leisuntgsdaten mit vorher gedrehtem Vorzeichen von i_temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kein Verstärker mit drehung VZ i_temp für positive P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicht-invertierender Verstärker und -i_temp, Übersteuern von i! </t>
   </si>
 </sst>
 </file>
@@ -472,13 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -716,7 +785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
@@ -727,13 +796,16 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -747,13 +819,16 @@
         <v>1000</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -767,13 +842,16 @@
         <v>1000</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -787,13 +865,16 @@
         <v>1000</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -807,13 +888,16 @@
         <v>1000</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -827,13 +911,16 @@
         <v>500</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -847,35 +934,64 @@
         <v>500</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>570</v>
+      </c>
+      <c r="D24">
+        <v>500</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24">
-        <v>570</v>
-      </c>
-      <c r="D24">
-        <v>500</v>
-      </c>
-      <c r="E24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>570</v>
+      </c>
+      <c r="D25">
+        <v>500</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
@@ -886,16 +1002,19 @@
       <c r="D26">
         <v>500</v>
       </c>
-      <c r="E26" t="s">
-        <v>35</v>
+      <c r="E26">
+        <v>4.7</v>
       </c>
       <c r="F26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
@@ -906,11 +1025,267 @@
       <c r="D27">
         <v>500</v>
       </c>
-      <c r="E27" t="s">
-        <v>35</v>
+      <c r="E27">
+        <v>-4.7</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>570</v>
+      </c>
+      <c r="D28">
+        <v>500</v>
+      </c>
+      <c r="E28">
+        <v>-4.7</v>
+      </c>
+      <c r="F28">
+        <v>7805</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>570</v>
+      </c>
+      <c r="D29">
+        <v>500</v>
+      </c>
+      <c r="E29">
+        <v>4.7</v>
+      </c>
+      <c r="F29">
+        <v>7805</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>570</v>
+      </c>
+      <c r="D30">
+        <v>500</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30">
+        <v>7805</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>570</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>570</v>
+      </c>
+      <c r="D33">
+        <v>500</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>570</v>
+      </c>
+      <c r="D34">
+        <v>500</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35">
+        <v>570</v>
+      </c>
+      <c r="D35">
+        <v>500</v>
+      </c>
+      <c r="E35">
+        <v>4.7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36">
+        <v>570</v>
+      </c>
+      <c r="D36">
+        <v>500</v>
+      </c>
+      <c r="E36">
+        <v>-4.7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <v>570</v>
+      </c>
+      <c r="D37">
+        <v>500</v>
+      </c>
+      <c r="E37">
+        <v>-4.7</v>
+      </c>
+      <c r="F37">
+        <v>7805</v>
+      </c>
+      <c r="G37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38">
+        <v>570</v>
+      </c>
+      <c r="D38">
+        <v>500</v>
+      </c>
+      <c r="E38">
+        <v>4.7</v>
+      </c>
+      <c r="F38">
+        <v>7805</v>
+      </c>
+      <c r="G38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39">
+        <v>570</v>
+      </c>
+      <c r="D39">
+        <v>500</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39">
+        <v>7805</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
versuch M und D miteinander zu lesen, funktioniert aber nicht. Neue Messreihen erstellt.
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="71">
   <si>
     <t>R1</t>
   </si>
@@ -197,6 +197,36 @@
   </si>
   <si>
     <t xml:space="preserve">nicht-invertierender Verstärker und -i_temp, Übersteuern von i! </t>
+  </si>
+  <si>
+    <t>ohne Verstärker</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>nicht-invertierender Verstärker</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>M17</t>
   </si>
 </sst>
 </file>
@@ -538,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,9 +1134,32 @@
         <v>51</v>
       </c>
     </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>570</v>
+      </c>
+      <c r="D31">
+        <v>500</v>
+      </c>
+      <c r="E31">
+        <v>3.2</v>
+      </c>
+      <c r="F31">
+        <v>7805</v>
+      </c>
+      <c r="G31" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1117,19 +1170,19 @@
       <c r="D32">
         <v>500</v>
       </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" t="s">
-        <v>36</v>
+      <c r="E32">
+        <v>-3.2</v>
+      </c>
+      <c r="F32">
+        <v>7805</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -1140,19 +1193,19 @@
       <c r="D33">
         <v>500</v>
       </c>
-      <c r="E33" t="s">
-        <v>34</v>
+      <c r="E33">
+        <v>-3.2</v>
       </c>
       <c r="F33" t="s">
         <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
@@ -1163,65 +1216,19 @@
       <c r="D34">
         <v>500</v>
       </c>
-      <c r="E34" t="s">
-        <v>34</v>
+      <c r="E34">
+        <v>3.2</v>
       </c>
       <c r="F34" t="s">
         <v>36</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35">
-        <v>570</v>
-      </c>
-      <c r="D35">
-        <v>500</v>
-      </c>
-      <c r="E35">
-        <v>4.7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36">
-        <v>570</v>
-      </c>
-      <c r="D36">
-        <v>500</v>
-      </c>
-      <c r="E36">
-        <v>-4.7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
@@ -1232,19 +1239,19 @@
       <c r="D37">
         <v>500</v>
       </c>
-      <c r="E37">
-        <v>-4.7</v>
-      </c>
-      <c r="F37">
-        <v>7805</v>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
@@ -1255,19 +1262,19 @@
       <c r="D38">
         <v>500</v>
       </c>
-      <c r="E38">
-        <v>4.7</v>
-      </c>
-      <c r="F38">
-        <v>7805</v>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
+        <v>36</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
         <v>23</v>
@@ -1281,11 +1288,218 @@
       <c r="E39" t="s">
         <v>34</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40">
+        <v>570</v>
+      </c>
+      <c r="D40">
+        <v>500</v>
+      </c>
+      <c r="E40">
+        <v>4.7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41">
+        <v>570</v>
+      </c>
+      <c r="D41">
+        <v>500</v>
+      </c>
+      <c r="E41">
+        <v>-4.7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>570</v>
+      </c>
+      <c r="D42">
+        <v>500</v>
+      </c>
+      <c r="E42">
+        <v>-4.7</v>
+      </c>
+      <c r="F42">
         <v>7805</v>
       </c>
-      <c r="G39" t="s">
-        <v>51</v>
+      <c r="G42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>570</v>
+      </c>
+      <c r="D43">
+        <v>500</v>
+      </c>
+      <c r="E43">
+        <v>4.7</v>
+      </c>
+      <c r="F43">
+        <v>7805</v>
+      </c>
+      <c r="G43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>570</v>
+      </c>
+      <c r="D44">
+        <v>500</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44">
+        <v>7805</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>570</v>
+      </c>
+      <c r="D45">
+        <v>500</v>
+      </c>
+      <c r="E45">
+        <v>3.2</v>
+      </c>
+      <c r="F45">
+        <v>7805</v>
+      </c>
+      <c r="G45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>570</v>
+      </c>
+      <c r="D46">
+        <v>500</v>
+      </c>
+      <c r="E46">
+        <v>-3.2</v>
+      </c>
+      <c r="F46">
+        <v>7805</v>
+      </c>
+      <c r="G46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47">
+        <v>570</v>
+      </c>
+      <c r="D47">
+        <v>500</v>
+      </c>
+      <c r="E47">
+        <v>-3.2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48">
+        <v>570</v>
+      </c>
+      <c r="D48">
+        <v>500</v>
+      </c>
+      <c r="E48">
+        <v>3.2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
programm anpassungen in Matlab, neue Messreihen
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
   <si>
     <t>R1</t>
   </si>
@@ -227,6 +227,27 @@
   </si>
   <si>
     <t>M17</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>M18</t>
+  </si>
+  <si>
+    <t>M19</t>
+  </si>
+  <si>
+    <t>2,7K</t>
+  </si>
+  <si>
+    <t>3V LM317 Spannungs teiler von U nicht auf 3V ausgelegt</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>3V LM317 U jetzt wieder voll ausgesteuert</t>
   </si>
 </sst>
 </file>
@@ -568,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,32 +1247,55 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37">
-        <v>570</v>
-      </c>
-      <c r="D37">
-        <v>500</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" t="s">
-        <v>57</v>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35">
+        <v>570</v>
+      </c>
+      <c r="D35">
+        <v>500</v>
+      </c>
+      <c r="E35">
+        <v>-5.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>500</v>
+      </c>
+      <c r="E36">
+        <v>-5.5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
@@ -1269,12 +1313,12 @@
         <v>36</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>23</v>
@@ -1292,12 +1336,12 @@
         <v>36</v>
       </c>
       <c r="G39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -1308,19 +1352,19 @@
       <c r="D40">
         <v>500</v>
       </c>
-      <c r="E40">
-        <v>4.7</v>
+      <c r="E40" t="s">
+        <v>34</v>
       </c>
       <c r="F40" t="s">
         <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
@@ -1332,18 +1376,18 @@
         <v>500</v>
       </c>
       <c r="E41">
-        <v>-4.7</v>
+        <v>4.7</v>
       </c>
       <c r="F41" t="s">
         <v>36</v>
       </c>
       <c r="G41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -1357,16 +1401,16 @@
       <c r="E42">
         <v>-4.7</v>
       </c>
-      <c r="F42">
-        <v>7805</v>
+      <c r="F42" t="s">
+        <v>36</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
@@ -1378,18 +1422,18 @@
         <v>500</v>
       </c>
       <c r="E43">
-        <v>4.7</v>
+        <v>-4.7</v>
       </c>
       <c r="F43">
         <v>7805</v>
       </c>
       <c r="G43" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
@@ -1400,19 +1444,19 @@
       <c r="D44">
         <v>500</v>
       </c>
-      <c r="E44" t="s">
-        <v>34</v>
+      <c r="E44">
+        <v>4.7</v>
       </c>
       <c r="F44">
         <v>7805</v>
       </c>
       <c r="G44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
@@ -1423,19 +1467,19 @@
       <c r="D45">
         <v>500</v>
       </c>
-      <c r="E45">
-        <v>3.2</v>
+      <c r="E45" t="s">
+        <v>34</v>
       </c>
       <c r="F45">
         <v>7805</v>
       </c>
       <c r="G45" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -1447,18 +1491,18 @@
         <v>500</v>
       </c>
       <c r="E46">
-        <v>-3.2</v>
+        <v>3.2</v>
       </c>
       <c r="F46">
         <v>7805</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
         <v>23</v>
@@ -1472,8 +1516,8 @@
       <c r="E47">
         <v>-3.2</v>
       </c>
-      <c r="F47" t="s">
-        <v>36</v>
+      <c r="F47">
+        <v>7805</v>
       </c>
       <c r="G47" t="s">
         <v>41</v>
@@ -1481,25 +1525,94 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48">
+        <v>570</v>
+      </c>
+      <c r="D48">
+        <v>500</v>
+      </c>
+      <c r="E48">
+        <v>-3.2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>69</v>
       </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48">
-        <v>570</v>
-      </c>
-      <c r="D48">
-        <v>500</v>
-      </c>
-      <c r="E48">
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49">
+        <v>570</v>
+      </c>
+      <c r="D49">
+        <v>500</v>
+      </c>
+      <c r="E49">
         <v>3.2</v>
       </c>
-      <c r="F48" t="s">
-        <v>36</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="F49" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50">
+        <v>570</v>
+      </c>
+      <c r="D50">
+        <v>500</v>
+      </c>
+      <c r="E50">
+        <v>-5.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51">
+        <v>100</v>
+      </c>
+      <c r="D51">
+        <v>500</v>
+      </c>
+      <c r="E51">
+        <v>-5.5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neues matlab analyse programm, Winkelbrechungen in Messreihen.xlsx hinzugefügt
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
   <si>
     <t>R1</t>
   </si>
@@ -248,12 +248,34 @@
   </si>
   <si>
     <t>3V LM317 U jetzt wieder voll ausgesteuert</t>
+  </si>
+  <si>
+    <t>Kap für (20°)</t>
+  </si>
+  <si>
+    <t>Phi bei 10µF</t>
+  </si>
+  <si>
+    <t>Phi bei 1µF</t>
+  </si>
+  <si>
+    <t>Ind für 20°</t>
+  </si>
+  <si>
+    <t>Phi bei 20mH</t>
+  </si>
+  <si>
+    <t>Phi bei 10mH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,8 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -589,18 +615,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -611,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -622,8 +654,32 @@
         <f>(1/G2)</f>
         <v>1.7825311942959001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <f xml:space="preserve"> TAN(20 * 180 / PI()) / (2*PI()*50*G2)</f>
+        <v>-5.4550386255249928E-6</v>
+      </c>
+      <c r="K2" s="2">
+        <f>ATAN(2*PI()*50*G2*0.00001) * 180 / PI()</f>
+        <v>60.429540482719482</v>
+      </c>
+      <c r="L2" s="2">
+        <f>ATAN(2*PI()*50*G2*0.000001) * 180 / PI()</f>
+        <v>9.9953526153809129</v>
+      </c>
+      <c r="M2" s="3">
+        <f xml:space="preserve"> TAN(20 / 180 *PI()) * G2 / (2*PI()*50)</f>
+        <v>0.64994836676238554</v>
+      </c>
+      <c r="N2" s="4">
+        <f>ATAN(2*PI()*50*0.02/G2)</f>
+        <v>1.1199505538784528E-2</v>
+      </c>
+      <c r="O2" s="4">
+        <f>ATAN(2*PI()*50*0.01/G2)</f>
+        <v>5.5999283676400639E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -634,8 +690,32 @@
         <f t="shared" ref="H3:H12" si="0">(1/G3)</f>
         <v>1.4598540145985401E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J12" si="1" xml:space="preserve"> TAN(20 * 180 / PI()) / (2*PI()*50*G3)</f>
+        <v>-4.4675571809044099E-5</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K12" si="2">ATAN(2*PI()*50*G3*0.00001) * 180 / PI()</f>
+        <v>12.144783119654919</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L12" si="3">ATAN(2*PI()*50*G3*0.000001) * 180 / PI()</f>
+        <v>1.2328097160935905</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M12" si="4" xml:space="preserve"> TAN(20 / 180 *PI()) * G3 /(2*PI()*50)</f>
+        <v>7.9360896832840311E-2</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" ref="N3:N12" si="5">ATAN(2*PI()*50*0.02/G3)</f>
+        <v>9.1469378982781097E-2</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:O12" si="6">ATAN(2*PI()*50*0.01/G3)</f>
+        <v>4.5830551393928394E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -649,8 +729,32 @@
         <f t="shared" si="0"/>
         <v>1.6393442622950821E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.016846998228723E-5</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="2"/>
+        <v>10.848473469707868</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0978656168493279</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="4"/>
+        <v>7.0671747544573116E-2</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="5"/>
+        <v>0.10264106472066194</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="6"/>
+        <v>5.1456056919296597E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -664,8 +768,32 @@
         <f t="shared" si="0"/>
         <v>2.865329512893983E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.7687010570759914E-5</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2570074654196555</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.62817482926174384</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="4"/>
+        <v>4.043350802140331E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="5"/>
+        <v>0.17812583512708408</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="6"/>
+        <v>8.9775019197857658E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -682,8 +810,32 @@
         <f t="shared" si="0"/>
         <v>3.0487804878048783E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>-9.3301117954863453E-5</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
+        <v>5.8832356764120464</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.59037910488047318</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8000546220688498E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="5"/>
+        <v>0.18926766992947311</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="6"/>
+        <v>9.5488973963880133E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -700,8 +852,32 @@
         <f t="shared" si="0"/>
         <v>4.2553191489361701E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.3022453910295834E-4</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>4.2223398458574257</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.42299231506178542</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="4"/>
+        <v>2.7226001103237189E-2</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.26125853075512323</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="6"/>
+        <v>0.13289683777362046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -721,8 +897,32 @@
         <f t="shared" si="0"/>
         <v>4.4444444444444446E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.3601229639642316E-4</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
+        <v>4.0432748919088857</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.40499325494445049</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="4"/>
+        <v>2.6067447864801561E-2</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.27231557938768775</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="6"/>
+        <v>0.13872944580142774</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -742,8 +942,32 @@
         <f t="shared" si="0"/>
         <v>5.6497175141242938E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.728969869446057E-4</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1827223233341093</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.31859671630555847</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="4"/>
+        <v>2.0506392320310561E-2</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="5"/>
+        <v>0.34110640996349428</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="6"/>
+        <v>0.17566172685973316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -766,8 +990,32 @@
         <f t="shared" si="0"/>
         <v>5.8139534883720929E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.7792306214648378E-4</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0929920097983943</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.30959698679466141</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="4"/>
+        <v>1.9927115701092749E-2</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="5"/>
+        <v>0.35024085905391994</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="6"/>
+        <v>0.18065929367775593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -790,8 +1038,32 @@
         <f t="shared" si="0"/>
         <v>7.0921985815602842E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.1704089850493056E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5363419506543989</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25379834001860385</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6335600661942312E-2</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="5"/>
+        <v>0.41920219603107528</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="6"/>
+        <v>0.21922707845215039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -817,21 +1089,64 @@
         <f t="shared" si="0"/>
         <v>7.2463768115942032E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.2175917890721167E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="2"/>
+        <v>2.4824454708705486</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24839844373569195</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5988034690411625E-2</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="5"/>
+        <v>0.42725537720896972</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="6"/>
+        <v>0.22383687519337153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>17</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Neue Messungen mit Kondensator
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
   <si>
     <t>R1</t>
   </si>
@@ -266,6 +266,42 @@
   </si>
   <si>
     <t>Phi bei 10mH</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>40µF parallel</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>30µF parallel</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>20µF parallel</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>10µF parallel</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>M21</t>
+  </si>
+  <si>
+    <t>M22</t>
+  </si>
+  <si>
+    <t>M23</t>
   </si>
 </sst>
 </file>
@@ -615,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,170 +1644,101 @@
         <v>77</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37">
+        <v>500</v>
+      </c>
+      <c r="E37">
+        <v>-5.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C38">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="D38">
         <v>500</v>
       </c>
-      <c r="E38" t="s">
-        <v>34</v>
+      <c r="E38">
+        <v>-5.5</v>
       </c>
       <c r="F38" t="s">
         <v>36</v>
       </c>
       <c r="G38" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C39">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="D39">
         <v>500</v>
       </c>
-      <c r="E39" t="s">
-        <v>34</v>
+      <c r="E39">
+        <v>-5.5</v>
       </c>
       <c r="F39" t="s">
         <v>36</v>
       </c>
       <c r="G39" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C40">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="D40">
         <v>500</v>
       </c>
-      <c r="E40" t="s">
-        <v>34</v>
+      <c r="E40">
+        <v>-5.5</v>
       </c>
       <c r="F40" t="s">
         <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41">
-        <v>570</v>
-      </c>
-      <c r="D41">
-        <v>500</v>
-      </c>
-      <c r="E41">
-        <v>4.7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>36</v>
-      </c>
-      <c r="G41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42">
-        <v>570</v>
-      </c>
-      <c r="D42">
-        <v>500</v>
-      </c>
-      <c r="E42">
-        <v>-4.7</v>
-      </c>
-      <c r="F42" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43">
-        <v>570</v>
-      </c>
-      <c r="D43">
-        <v>500</v>
-      </c>
-      <c r="E43">
-        <v>-4.7</v>
-      </c>
-      <c r="F43">
-        <v>7805</v>
-      </c>
-      <c r="G43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44">
-        <v>570</v>
-      </c>
-      <c r="D44">
-        <v>500</v>
-      </c>
-      <c r="E44">
-        <v>4.7</v>
-      </c>
-      <c r="F44">
-        <v>7805</v>
-      </c>
-      <c r="G44" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
@@ -1785,16 +1752,16 @@
       <c r="E45" t="s">
         <v>34</v>
       </c>
-      <c r="F45">
-        <v>7805</v>
+      <c r="F45" t="s">
+        <v>36</v>
       </c>
       <c r="G45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -1805,19 +1772,19 @@
       <c r="D46">
         <v>500</v>
       </c>
-      <c r="E46">
-        <v>3.2</v>
-      </c>
-      <c r="F46">
-        <v>7805</v>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" t="s">
+        <v>36</v>
       </c>
       <c r="G46" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
         <v>23</v>
@@ -1828,19 +1795,19 @@
       <c r="D47">
         <v>500</v>
       </c>
-      <c r="E47">
-        <v>-3.2</v>
-      </c>
-      <c r="F47">
-        <v>7805</v>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" t="s">
+        <v>36</v>
       </c>
       <c r="G47" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
         <v>23</v>
@@ -1852,18 +1819,18 @@
         <v>500</v>
       </c>
       <c r="E48">
-        <v>-3.2</v>
+        <v>4.7</v>
       </c>
       <c r="F48" t="s">
         <v>36</v>
       </c>
       <c r="G48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -1875,18 +1842,18 @@
         <v>500</v>
       </c>
       <c r="E49">
-        <v>3.2</v>
+        <v>-4.7</v>
       </c>
       <c r="F49" t="s">
         <v>36</v>
       </c>
       <c r="G49" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
         <v>23</v>
@@ -1898,36 +1865,289 @@
         <v>500</v>
       </c>
       <c r="E50">
-        <v>-5.5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>36</v>
+        <v>-4.7</v>
+      </c>
+      <c r="F50">
+        <v>7805</v>
       </c>
       <c r="G50" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>570</v>
+      </c>
+      <c r="D51">
+        <v>500</v>
+      </c>
+      <c r="E51">
+        <v>4.7</v>
+      </c>
+      <c r="F51">
+        <v>7805</v>
+      </c>
+      <c r="G51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52">
+        <v>570</v>
+      </c>
+      <c r="D52">
+        <v>500</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52">
+        <v>7805</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53">
+        <v>570</v>
+      </c>
+      <c r="D53">
+        <v>500</v>
+      </c>
+      <c r="E53">
+        <v>3.2</v>
+      </c>
+      <c r="F53">
+        <v>7805</v>
+      </c>
+      <c r="G53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54">
+        <v>570</v>
+      </c>
+      <c r="D54">
+        <v>500</v>
+      </c>
+      <c r="E54">
+        <v>-3.2</v>
+      </c>
+      <c r="F54">
+        <v>7805</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55">
+        <v>570</v>
+      </c>
+      <c r="D55">
+        <v>500</v>
+      </c>
+      <c r="E55">
+        <v>-3.2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56">
+        <v>570</v>
+      </c>
+      <c r="D56">
+        <v>500</v>
+      </c>
+      <c r="E56">
+        <v>3.2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57">
+        <v>570</v>
+      </c>
+      <c r="D57">
+        <v>500</v>
+      </c>
+      <c r="E57">
+        <v>-5.5</v>
+      </c>
+      <c r="F57" t="s">
+        <v>36</v>
+      </c>
+      <c r="G57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>76</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B58" t="s">
         <v>74</v>
       </c>
-      <c r="C51">
+      <c r="C58">
         <v>100</v>
       </c>
-      <c r="D51">
-        <v>500</v>
-      </c>
-      <c r="E51">
+      <c r="D58">
+        <v>500</v>
+      </c>
+      <c r="E58">
         <v>-5.5</v>
       </c>
-      <c r="F51" t="s">
-        <v>36</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="F58" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59">
+        <v>500</v>
+      </c>
+      <c r="E59">
+        <v>-5.5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60">
+        <v>100</v>
+      </c>
+      <c r="D60">
+        <v>500</v>
+      </c>
+      <c r="E60">
+        <v>-5.5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61">
+        <v>100</v>
+      </c>
+      <c r="D61">
+        <v>500</v>
+      </c>
+      <c r="E61">
+        <v>-5.5</v>
+      </c>
+      <c r="F61" t="s">
+        <v>36</v>
+      </c>
+      <c r="G61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62">
+        <v>100</v>
+      </c>
+      <c r="D62">
+        <v>500</v>
+      </c>
+      <c r="E62">
+        <v>-5.5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>36</v>
+      </c>
+      <c r="G62" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Messreihen.xlsx erneuert VCC VREF
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="117">
   <si>
     <t>R1</t>
   </si>
@@ -329,6 +329,42 @@
   </si>
   <si>
     <t>zwei mal I (mit und ohne Verstärkung)</t>
+  </si>
+  <si>
+    <t>VCC01</t>
+  </si>
+  <si>
+    <t>VCC mit CPU, ohne Kondensator</t>
+  </si>
+  <si>
+    <t>VCC ohne CPU, ohne Kondensator</t>
+  </si>
+  <si>
+    <t>VCC02</t>
+  </si>
+  <si>
+    <t>VCC03</t>
+  </si>
+  <si>
+    <t>VCC mit CPU, mit Kondensator</t>
+  </si>
+  <si>
+    <t>VCC ohne CPU, mit Kondensator</t>
+  </si>
+  <si>
+    <t>VCC04</t>
+  </si>
+  <si>
+    <t>VREF von LM317 3,1V</t>
+  </si>
+  <si>
+    <t>VREF01</t>
+  </si>
+  <si>
+    <t>VREF02</t>
+  </si>
+  <si>
+    <t>VREF von AREF Pin µC</t>
   </si>
 </sst>
 </file>
@@ -678,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,6 +2374,54 @@
         <v>104</v>
       </c>
     </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>105</v>
+      </c>
+      <c r="G72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G73" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>109</v>
+      </c>
+      <c r="G74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>114</v>
+      </c>
+      <c r="G77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>115</v>
+      </c>
+      <c r="G78" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Neue Messreihe mit Hallsensor
</commit_message>
<xml_diff>
--- a/Matlab/Messreihen.xlsx
+++ b/Matlab/Messreihen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="128">
   <si>
     <t>R1</t>
   </si>
@@ -386,6 +386,18 @@
   </si>
   <si>
     <t>VREF umschalten ohne Stüzkondensator</t>
+  </si>
+  <si>
+    <t>W07</t>
+  </si>
+  <si>
+    <t>I von Hallsensor gemessen</t>
+  </si>
+  <si>
+    <t>W08</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -735,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,83 +2407,114 @@
         <v>104</v>
       </c>
     </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="G71" t="s">
+        <v>127</v>
+      </c>
+    </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>105</v>
+        <v>126</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72">
+        <v>100</v>
+      </c>
+      <c r="D72">
+        <v>500</v>
+      </c>
+      <c r="E72">
+        <v>-5.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>36</v>
       </c>
       <c r="G72" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G73" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>109</v>
-      </c>
-      <c r="G74" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G75" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>108</v>
+      </c>
+      <c r="G76" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G77" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G78" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>117</v>
-      </c>
-      <c r="G79" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G80" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G81" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>115</v>
+      </c>
+      <c r="G83" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>120</v>
+      </c>
+      <c r="G84" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>122</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G85" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>